<commit_message>
bf: update preatas forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Burkina Faso/2024/bf_lf_pretas_202404_2_Enrolement.xlsx
+++ b/LF/PreTAS/Burkina Faso/2024/bf_lf_pretas_202404_2_Enrolement.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Burkina Faso\2024\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C4E79C-50F7-422E-9642-1F3A581A5902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="183">
   <si>
     <t>type</t>
   </si>
@@ -192,9 +198,6 @@
     <t>Numéro enquêté (${p_recorder_id}${p_Numero_famille}...)</t>
   </si>
   <si>
-    <t>regex(., '^[0-9]{2}$')</t>
-  </si>
-  <si>
     <t>Entrer uniquement les trois derniers chiffre du numéro enquété</t>
   </si>
   <si>
@@ -570,31 +573,32 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(BF - Dec 2022) Pré TAS FL - 2. Formulaire Enrôlement V2</t>
-  </si>
-  <si>
-    <t>bf_lf_pretas_2_Enrolement_2022 061222_v2</t>
-  </si>
-  <si>
     <t>French</t>
+  </si>
+  <si>
+    <t>bf_lf_pretas_202404_2_Enrolement</t>
+  </si>
+  <si>
+    <t>(BF - Apr 2024) Pré TAS FL - 2. Formulaire Enrôlement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -628,152 +632,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -794,13 +654,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,176 +670,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -989,354 +681,63 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
+        <color theme="0" tint="-0.14990691854609822"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
+        <color theme="0" tint="-0.14990691854609822"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
+        <color theme="0" tint="-0.14990691854609822"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.149937437055574"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="0" tint="-0.14990691854609822"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
       </font>
       <fill>
@@ -1356,20 +757,23 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
-      <color rgb="0066CCFF"/>
-      <color rgb="00FFFFCC"/>
+      <color rgb="FF66CCFF"/>
+      <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1627,68 +1031,68 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.4166666666667" customWidth="1"/>
-    <col min="2" max="2" width="19.6833333333333" customWidth="1"/>
-    <col min="3" max="3" width="57.4166666666667" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="11.4166666666667" customWidth="1"/>
-    <col min="6" max="6" width="36.625" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="20.8916666666667" customWidth="1"/>
-    <col min="9" max="9" width="33.6833333333333" customWidth="1"/>
-    <col min="11" max="11" width="41.1" customWidth="1"/>
-    <col min="13" max="13" width="13.6833333333333" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="7" max="7" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="41.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="1" ht="18" spans="1:14">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="18.75">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="7" t="s">
@@ -1698,7 +1102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1712,8 +1116,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
@@ -1726,89 +1130,89 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:14" ht="30">
+      <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="10" t="s">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="17"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="10" t="s">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="10" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" ht="28.5" spans="1:10">
-      <c r="A8" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:14" ht="30">
+      <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B8" t="s">
@@ -1824,8 +1228,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
@@ -1841,8 +1245,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
@@ -1867,8 +1271,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:14">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
@@ -1893,104 +1297,104 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:14">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="17"/>
-    </row>
-    <row r="13" ht="32.7" customHeight="1" spans="1:13">
-      <c r="A13" s="10" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:14" ht="32.65" customHeight="1">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:14" ht="60">
+      <c r="A14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="C14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="17"/>
-    </row>
-    <row r="14" ht="57" spans="1:14">
-      <c r="A14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="17"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="14"/>
       <c r="N14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>62</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>63</v>
-      </c>
-      <c r="G15" t="s">
-        <v>64</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -1999,15 +1403,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2017,14 +1421,14 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>69</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
       </c>
       <c r="H17" t="s">
         <v>33</v>
@@ -2033,57 +1437,57 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" s="8" customFormat="1" spans="1:10">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" ht="28.5" spans="1:10">
-      <c r="A19" s="13" t="s">
+      <c r="B19" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="15" t="s">
-        <v>77</v>
       </c>
       <c r="J19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:10" ht="30">
+      <c r="A20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
       </c>
       <c r="H20" t="s">
         <v>33</v>
@@ -2092,31 +1496,31 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="H21" t="s">
         <v>82</v>
       </c>
-      <c r="H21" t="s">
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>84</v>
       </c>
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="13" t="s">
         <v>33</v>
       </c>
       <c r="J22" t="s">
@@ -2124,93 +1528,91 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
       </c>
-      <c r="C23" t="s">
+      <c r="H23" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>88</v>
       </c>
       <c r="J23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
         <v>89</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>90</v>
       </c>
-      <c r="C24" t="s">
+      <c r="H24" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H24" s="16" t="s">
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="10" t="s">
+      <c r="B25" t="s">
         <v>93</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>94</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>96</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="10" t="s">
+      <c r="B27" t="s">
         <v>98</v>
       </c>
-      <c r="B27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="10"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.3166666666667" customWidth="1"/>
-    <col min="2" max="2" width="39.6833333333333" customWidth="1"/>
-    <col min="3" max="3" width="19.1" customWidth="1"/>
-    <col min="5" max="5" width="11.525" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2219,467 +1621,465 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
         <v>108</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
         <v>110</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>112</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="10" s="2" customFormat="1" spans="1:1">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="B13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>125</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>127</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>129</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>130</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>132</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>134</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>135</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>137</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>139</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>140</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>142</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>144</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
+      <c r="B27" t="s">
         <v>151</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>152</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>154</v>
-      </c>
-      <c r="C28" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>177</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
     <sortCondition ref="A10:A28"/>
     <sortCondition ref="B10:B28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="1" max="1" width="56" style="16" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bf: update pretas form for BF.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Burkina Faso/2024/bf_lf_pretas_202404_2_Enrolement.xlsx
+++ b/LF/PreTAS/Burkina Faso/2024/bf_lf_pretas_202404_2_Enrolement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Burkina Faso\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E890DCF3-1D4C-4386-8D6D-C45D55F036BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B685DEF-282B-4D96-9789-310B152B8134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="216">
   <si>
     <t>type</t>
   </si>
@@ -237,9 +237,6 @@
     <t>p_migration</t>
   </si>
   <si>
-    <t>p_migration (personnes entrée il y a moins 5 ans d'un pays voisin ou autre localités)</t>
-  </si>
-  <si>
     <t>p_migration_autre</t>
   </si>
   <si>
@@ -667,6 +664,12 @@
   </si>
   <si>
     <t>. &lt;= ${p_age_yrs}</t>
+  </si>
+  <si>
+    <t>Migration (personnes entrée il y a moins 5 ans d'un pays voisin ou autre localités)</t>
+  </si>
+  <si>
+    <t>${p_deja_ete_traiter_par_ivm_alb}='1_oui' and ${p_consent} = '1_oui'</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1161,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1429,7 +1432,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>50</v>
@@ -1459,10 +1462,10 @@
         <v>53</v>
       </c>
       <c r="F13" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>206</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>33</v>
@@ -1546,10 +1549,10 @@
         <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>33</v>
@@ -1560,13 +1563,13 @@
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1581,13 +1584,13 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="8" t="s">
         <v>187</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1605,10 +1608,10 @@
         <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>190</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1626,18 +1629,18 @@
         <v>57</v>
       </c>
       <c r="B21" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>33</v>
@@ -1651,21 +1654,21 @@
         <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="G22" s="21" t="s">
-        <v>210</v>
-      </c>
       <c r="H22" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>17</v>
@@ -1676,10 +1679,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -1706,8 +1709,8 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="3" t="s">
-        <v>33</v>
+      <c r="H24" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>17</v>
@@ -1718,17 +1721,17 @@
         <v>68</v>
       </c>
       <c r="B25" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>211</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>212</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>17</v>
@@ -1741,8 +1744,8 @@
       <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>71</v>
+      <c r="C26" s="20" t="s">
+        <v>214</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>33</v>
@@ -1756,13 +1759,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1770,10 +1773,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>33</v>
@@ -1787,13 +1790,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="H29" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>17</v>
@@ -1801,43 +1804,43 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="H30" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1869,7 +1872,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
@@ -1878,101 +1881,101 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>96</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
@@ -1980,445 +1983,445 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>110</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="C25" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="C32" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B34" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B35" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>155</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B36" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>157</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B37" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>159</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2447,24 +2450,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>208</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>